<commit_message>
Add alarm and notification.
</commit_message>
<xml_diff>
--- a/StudyProgress/Ebbinghaus-Android.xlsx
+++ b/StudyProgress/Ebbinghaus-Android.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="30" windowWidth="19200" windowHeight="9825"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$1:$4</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -74,10 +74,6 @@
   </si>
   <si>
     <t>艾宾浩斯遗忘曲线复习计划表</t>
-    <phoneticPr fontId="22" type="noConversion"/>
-  </si>
-  <si>
-    <t>第一章，第二章</t>
     <phoneticPr fontId="22" type="noConversion"/>
   </si>
   <si>
@@ -295,6 +291,10 @@
   </si>
   <si>
     <t>20 耳洞</t>
+    <phoneticPr fontId="22" type="noConversion"/>
+  </si>
+  <si>
+    <t>第一章，13-序列化（S， Parcelable），定时任务（Timer，Alarm），PendingIntent，Notification</t>
     <phoneticPr fontId="22" type="noConversion"/>
   </si>
 </sst>
@@ -1043,6 +1043,12 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1065,12 +1071,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1486,101 +1486,101 @@
   <dimension ref="A1:Q369"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="5.75" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="1" customWidth="1"/>
-    <col min="3" max="3" width="64" customWidth="1"/>
+    <col min="3" max="3" width="92" customWidth="1"/>
     <col min="4" max="14" width="5.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="51" customHeight="1">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
     </row>
     <row r="2" spans="1:17" ht="21.75" customHeight="1">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="19" t="s">
+      <c r="P2" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="P2" s="19" t="s">
+      <c r="Q2" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="Q2" s="19" t="s">
+    </row>
+    <row r="3" spans="1:17" ht="41.25" customHeight="1">
+      <c r="A3" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="19" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" ht="41.25" customHeight="1">
-      <c r="A3" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="27"/>
-      <c r="O3" s="19" t="s">
+      <c r="P3" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="P3" s="19" t="s">
-        <v>36</v>
-      </c>
       <c r="Q3" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="47.25" customHeight="1">
-      <c r="A4" s="24"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="24"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="26"/>
       <c r="D4" s="3" t="s">
         <v>5</v>
       </c>
@@ -1615,13 +1615,13 @@
         <v>15</v>
       </c>
       <c r="O4" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P4" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q4" s="20" t="s">
         <v>43</v>
-      </c>
-      <c r="Q4" s="20" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="24.95" customHeight="1">
@@ -1629,10 +1629,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="18">
-        <v>43402</v>
+        <v>43413</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="D5" s="13">
         <f>A5</f>
@@ -1671,13 +1671,13 @@
         <v>17</v>
       </c>
       <c r="O5" s="21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="P5" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q5" s="21" t="s">
         <v>38</v>
-      </c>
-      <c r="Q5" s="21" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="24.95" customHeight="1">
@@ -1686,10 +1686,10 @@
       </c>
       <c r="B6" s="9">
         <f>B5+1</f>
-        <v>43403</v>
+        <v>43414</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D6" s="7">
         <f t="shared" ref="D6:D69" si="0">A6</f>
@@ -1728,13 +1728,13 @@
         <v>17</v>
       </c>
       <c r="O6" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="P6" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="P6" s="21" t="s">
-        <v>41</v>
-      </c>
       <c r="Q6" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="24.95" customHeight="1">
@@ -1743,10 +1743,10 @@
       </c>
       <c r="B7" s="9">
         <f t="shared" ref="B7:B16" si="3">B6+1</f>
-        <v>43404</v>
+        <v>43415</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" s="7">
         <f t="shared" si="0"/>
@@ -1785,13 +1785,13 @@
         <v>17</v>
       </c>
       <c r="O7" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="P7" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="P7" s="21" t="s">
+      <c r="Q7" s="21" t="s">
         <v>48</v>
-      </c>
-      <c r="Q7" s="21" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="24.95" customHeight="1">
@@ -1800,10 +1800,10 @@
       </c>
       <c r="B8" s="9">
         <f t="shared" si="3"/>
-        <v>43405</v>
+        <v>43416</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" s="7">
         <f t="shared" si="0"/>
@@ -1841,14 +1841,14 @@
       <c r="N8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="O8" s="30" t="s">
+      <c r="O8" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="P8" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="P8" s="31" t="s">
+      <c r="Q8" s="23" t="s">
         <v>51</v>
-      </c>
-      <c r="Q8" s="31" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="24.95" customHeight="1">
@@ -1857,10 +1857,10 @@
       </c>
       <c r="B9" s="9">
         <f t="shared" si="3"/>
-        <v>43406</v>
+        <v>43417</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" s="7">
         <f t="shared" si="0"/>
@@ -1905,10 +1905,10 @@
       </c>
       <c r="B10" s="9">
         <f t="shared" si="3"/>
-        <v>43407</v>
+        <v>43418</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D10" s="7">
         <f t="shared" si="0"/>
@@ -1953,10 +1953,10 @@
       </c>
       <c r="B11" s="9">
         <f t="shared" si="3"/>
-        <v>43408</v>
+        <v>43419</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" s="7">
         <f t="shared" si="0"/>
@@ -2001,10 +2001,10 @@
       </c>
       <c r="B12" s="9">
         <f t="shared" si="3"/>
-        <v>43409</v>
+        <v>43420</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" s="7">
         <f t="shared" si="0"/>
@@ -2049,10 +2049,10 @@
       </c>
       <c r="B13" s="9">
         <f t="shared" si="3"/>
-        <v>43410</v>
+        <v>43421</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13" s="7">
         <f t="shared" si="0"/>
@@ -2097,10 +2097,10 @@
       </c>
       <c r="B14" s="9">
         <f t="shared" si="3"/>
-        <v>43411</v>
+        <v>43422</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D14" s="7">
         <f t="shared" si="0"/>
@@ -2145,10 +2145,10 @@
       </c>
       <c r="B15" s="9">
         <f t="shared" si="3"/>
-        <v>43412</v>
+        <v>43423</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D15" s="7">
         <f t="shared" si="0"/>
@@ -2193,10 +2193,10 @@
       </c>
       <c r="B16" s="9">
         <f t="shared" si="3"/>
-        <v>43413</v>
+        <v>43424</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D16" s="7">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Receive boot complete ok.
</commit_message>
<xml_diff>
--- a/StudyProgress/Ebbinghaus-Android.xlsx
+++ b/StudyProgress/Ebbinghaus-Android.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="30" windowWidth="19200" windowHeight="9825"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$1:$4</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -81,14 +81,6 @@
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
   <si>
-    <t>07 内容提供者 08 多媒体</t>
-    <phoneticPr fontId="21" type="noConversion"/>
-  </si>
-  <si>
-    <t>09 网络 10 服务</t>
-    <phoneticPr fontId="21" type="noConversion"/>
-  </si>
-  <si>
     <t>06数据存储-（文件，SharedPreference） 
 13-序列化（S， Parcelable），定时任务（Timer，Alarm）</t>
     <phoneticPr fontId="21" type="noConversion"/>
@@ -101,6 +93,14 @@
   </si>
   <si>
     <t>01羚羊 02灵儿 03灵山 04零食 05领悟 06领路 07邦德 08葫芦 09菱角 10棒球 11筷子 12婴儿 13医生 14钥匙 15鹦鹉 16杨柳 17仪器 18泥巴 19药酒 20耳洞</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>09 网络</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>07 内容提供者 08 多媒体 10 服务</t>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
 </sst>
@@ -812,6 +812,9 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -835,9 +838,6 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1252,7 +1252,7 @@
   <dimension ref="A1:N369"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1264,71 +1264,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="51" customHeight="1">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
     </row>
     <row r="2" spans="1:14" ht="21.75" customHeight="1">
-      <c r="A2" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
+      <c r="A2" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
     </row>
     <row r="3" spans="1:14" ht="41.25" customHeight="1">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="22" t="s">
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="25"/>
     </row>
     <row r="4" spans="1:14" ht="47.25" customHeight="1">
-      <c r="A4" s="21"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="21"/>
+      <c r="A4" s="22"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="22"/>
       <c r="D4" s="3" t="s">
         <v>5</v>
       </c>
@@ -1370,8 +1370,8 @@
       <c r="B5" s="17">
         <v>43413</v>
       </c>
-      <c r="C5" s="27" t="s">
-        <v>22</v>
+      <c r="C5" s="19" t="s">
+        <v>20</v>
       </c>
       <c r="D5" s="12">
         <f>A5</f>
@@ -1418,8 +1418,8 @@
         <f>B5+1</f>
         <v>43414</v>
       </c>
-      <c r="C6" s="27" t="s">
-        <v>23</v>
+      <c r="C6" s="19" t="s">
+        <v>21</v>
       </c>
       <c r="D6" s="12">
         <f t="shared" ref="D6:D69" si="0">A6</f>
@@ -1510,29 +1510,29 @@
       <c r="A8" s="4">
         <v>4</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="17">
         <f t="shared" si="3"/>
         <v>43416</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="7">
+      <c r="C8" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="12">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="12">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="12">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="12">
         <v>3</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="12">
         <v>2</v>
       </c>
       <c r="I8" s="7" t="s">
@@ -1563,7 +1563,7 @@
         <v>43417</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D9" s="7">
         <f t="shared" si="0"/>

</xml_diff>